<commit_message>
Solomon - Level 2 done
</commit_message>
<xml_diff>
--- a/trunk/SolomonsKey/Solomon.xlsx
+++ b/trunk/SolomonsKey/Solomon.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>1-1</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>Room 1 Enter door</t>
+  </si>
+  <si>
+    <t>Room 2 1st move</t>
+  </si>
+  <si>
+    <t>Room 2 Get key</t>
+  </si>
+  <si>
+    <t>Room 3 1st move</t>
+  </si>
+  <si>
+    <t>Room 2 Enter door</t>
   </si>
 </sst>
 </file>
@@ -573,7 +585,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -635,27 +647,63 @@
       </c>
     </row>
     <row r="5" spans="1:4">
+      <c r="A5" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="16">
+        <v>1553</v>
+      </c>
+      <c r="C5" s="16">
+        <v>1650</v>
+      </c>
       <c r="D5" s="16">
         <f t="shared" ref="D5:D68" si="0">IF(B5 &gt;  0,C5-B5-$D$3, 0)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="6" spans="1:4">
+      <c r="A6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="16">
+        <v>1899</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1989</v>
+      </c>
       <c r="D6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="7" spans="1:4">
+      <c r="A7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C7" s="16">
+        <v>2116</v>
+      </c>
       <c r="D7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="8" spans="1:4">
+      <c r="A8" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="16">
+        <v>2740</v>
+      </c>
+      <c r="C8" s="16">
+        <v>2833</v>
+      </c>
       <c r="D8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="9" spans="1:4">

</xml_diff>

<commit_message>
Replaced main .fm2 with Randil's wip.  I attempted to continue level 3 but epic fail.
</commit_message>
<xml_diff>
--- a/trunk/SolomonsKey/Solomon.xlsx
+++ b/trunk/SolomonsKey/Solomon.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>1-1</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>Room 2 Enter door</t>
+  </si>
+  <si>
+    <t>Room 1 1st move</t>
+  </si>
+  <si>
+    <t>Room 3 Destroy 1st block</t>
+  </si>
+  <si>
+    <t>Room 3 Land</t>
+  </si>
+  <si>
+    <t>Bust 1st block at bottom</t>
   </si>
 </sst>
 </file>
@@ -213,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -250,11 +262,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -286,7 +307,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,20 +603,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.7109375" style="16" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="16"/>
+    <col min="2" max="6" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>40</v>
       </c>
@@ -607,16 +629,24 @@
       <c r="D1" s="14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="13" customFormat="1" ht="19.5" thickTop="1">
+      <c r="E1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
       <c r="A2" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
         <v>45</v>
       </c>
@@ -630,709 +660,1213 @@
         <f>IF(B3 &gt;  0,C3-B3, 0)</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="16" t="s">
-        <v>46</v>
+      <c r="E3" s="16">
+        <v>36</v>
+      </c>
+      <c r="F3" s="16">
+        <f>IF(B3 &gt;  0,E3-B3, 0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="B4" s="16">
-        <v>836</v>
+        <v>332</v>
       </c>
       <c r="C4" s="16">
-        <v>931</v>
+        <v>433</v>
       </c>
       <c r="D4" s="16">
         <f>IF(B4 &gt;  0,C4-B4-$D$3, 0)</f>
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16">
+        <v>336</v>
+      </c>
+      <c r="F4" s="16">
+        <f t="shared" ref="F4:F67" si="0">IF(B4 &gt;  0,E4-B4, 0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="16">
+        <v>829</v>
+      </c>
+      <c r="C5" s="16">
+        <v>931</v>
+      </c>
+      <c r="D5" s="16">
+        <f>IF(B5 &gt;  0,C5-B5-$D$3, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="16">
+        <v>833</v>
+      </c>
+      <c r="F5" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="16">
-        <v>1553</v>
-      </c>
-      <c r="C5" s="16">
+      <c r="B6" s="16">
+        <v>1547</v>
+      </c>
+      <c r="C6" s="16">
         <v>1650</v>
       </c>
-      <c r="D5" s="16">
-        <f t="shared" ref="D5:D68" si="0">IF(B5 &gt;  0,C5-B5-$D$3, 0)</f>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="16" t="s">
+      <c r="D6" s="16">
+        <f t="shared" ref="D6:D69" si="1">IF(B6 &gt;  0,C6-B6-$D$3, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1551</v>
+      </c>
+      <c r="F6" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="16">
-        <v>1899</v>
-      </c>
-      <c r="C6" s="16">
+      <c r="B7" s="16">
+        <v>1884</v>
+      </c>
+      <c r="C7" s="16">
         <v>1989</v>
       </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="16" t="s">
+      <c r="D7" s="16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1889</v>
+      </c>
+      <c r="F7" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="16">
-        <v>2023</v>
-      </c>
-      <c r="C7" s="16">
+      <c r="B8" s="16">
+        <v>2011</v>
+      </c>
+      <c r="C8" s="16">
         <v>2116</v>
       </c>
-      <c r="D7" s="16">
-        <f t="shared" si="0"/>
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="16" t="s">
+      <c r="D8" s="16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E8" s="16">
+        <v>2016</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="16">
-        <v>2740</v>
-      </c>
-      <c r="C8" s="16">
+      <c r="B9" s="16">
+        <v>2728</v>
+      </c>
+      <c r="C9" s="16">
         <v>2833</v>
       </c>
-      <c r="D8" s="16">
-        <f t="shared" si="0"/>
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
       <c r="D9" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E9" s="16">
+        <v>2733</v>
+      </c>
+      <c r="F9" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="16">
+        <v>2821</v>
+      </c>
+      <c r="C10" s="16">
+        <v>2924</v>
+      </c>
       <c r="D10" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F10" s="16">
+        <f t="shared" si="0"/>
+        <v>-2821</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="16">
+        <v>3188</v>
+      </c>
+      <c r="C11" s="16">
+        <v>3304</v>
+      </c>
       <c r="D11" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="0"/>
+        <v>-3188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="16">
+        <v>3370</v>
+      </c>
       <c r="D12" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="D13" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="D14" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="D15" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="D16" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6">
       <c r="D17" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6">
       <c r="D18" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6">
       <c r="D19" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6">
       <c r="D20" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6">
       <c r="D21" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6">
       <c r="D22" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6">
       <c r="D23" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6">
       <c r="D24" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6">
       <c r="D25" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6">
       <c r="D26" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6">
       <c r="D27" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6">
       <c r="D28" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6">
       <c r="D29" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6">
       <c r="D30" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6">
       <c r="D31" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6">
       <c r="D32" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6">
       <c r="D33" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6">
       <c r="D34" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6">
       <c r="D35" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6">
       <c r="D36" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6">
       <c r="D37" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6">
       <c r="D38" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6">
       <c r="D39" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6">
       <c r="D40" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6">
       <c r="D41" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6">
       <c r="D42" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6">
       <c r="D43" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6">
       <c r="D44" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6">
       <c r="D45" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F45" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6">
       <c r="D46" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6">
       <c r="D47" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6">
       <c r="D48" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6">
       <c r="D49" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6">
       <c r="D50" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6">
       <c r="D51" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6">
       <c r="D52" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6">
       <c r="D53" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6">
       <c r="D54" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6">
       <c r="D55" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6">
       <c r="D56" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6">
       <c r="D57" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6">
       <c r="D58" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="4:6">
       <c r="D59" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6">
       <c r="D60" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6">
       <c r="D61" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6">
       <c r="D62" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="4:6">
       <c r="D63" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="4:6">
       <c r="D64" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F64" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6">
       <c r="D65" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6">
       <c r="D66" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6">
       <c r="D67" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F67" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6">
       <c r="D68" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F68" s="16">
+        <f t="shared" ref="F68:F113" si="2">IF(B68 &gt;  0,E68-B68, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="4:6">
       <c r="D69" s="16">
-        <f t="shared" ref="D69:D112" si="1">IF(B69 &gt;  0,C69-B69-$D$3, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="4:4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F69" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="4:6">
       <c r="D70" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="4:4">
+        <f t="shared" ref="D70:D113" si="3">IF(B70 &gt;  0,C70-B70-$D$3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F70" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="4:6">
       <c r="D71" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F71" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="4:6">
       <c r="D72" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F72" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="4:6">
       <c r="D73" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F73" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="4:6">
       <c r="D74" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F74" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="4:6">
       <c r="D75" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F75" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="4:6">
       <c r="D76" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F76" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="4:6">
       <c r="D77" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F77" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="4:6">
       <c r="D78" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F78" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="4:6">
       <c r="D79" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F79" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="4:6">
       <c r="D80" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F80" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="4:6">
       <c r="D81" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F81" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="4:6">
       <c r="D82" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F82" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6">
       <c r="D83" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F83" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="4:6">
       <c r="D84" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F84" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="4:6">
       <c r="D85" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F85" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6">
       <c r="D86" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F86" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="4:6">
       <c r="D87" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F87" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="4:6">
       <c r="D88" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F88" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="4:6">
       <c r="D89" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F89" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6">
       <c r="D90" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F90" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="4:6">
       <c r="D91" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F91" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="4:6">
       <c r="D92" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F92" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="4:6">
       <c r="D93" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F93" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="4:6">
       <c r="D94" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F94" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="4:6">
       <c r="D95" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F95" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="4:6">
       <c r="D96" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F96" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6">
       <c r="D97" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F97" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6">
       <c r="D98" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F98" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="4:6">
       <c r="D99" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F99" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6">
       <c r="D100" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F100" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6">
       <c r="D101" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F101" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="4:6">
       <c r="D102" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F102" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="4:6">
       <c r="D103" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F103" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="4:6">
       <c r="D104" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F104" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="4:6">
       <c r="D105" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F105" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="4:6">
       <c r="D106" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F106" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="4:6">
       <c r="D107" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F107" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="4:6">
       <c r="D108" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F108" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="4:6">
       <c r="D109" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F109" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="4:6">
       <c r="D110" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F110" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="4:6">
       <c r="D111" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="4:4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F111" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="4:6">
       <c r="D112" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F112" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="4:6">
+      <c r="D113" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F113" s="16">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>